<commit_message>
Docs | Fix | item_list.xlxs : is_sell Column 값 수정
is_sell 부분을 true, false 에서 => 1, 0으로 교체
Sqlite3에서 true, false를 인식못하기 때문에
</commit_message>
<xml_diff>
--- a/public/resource/exel/item_list.xlsx
+++ b/public/resource/exel/item_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021C7520-9EC2-475A-A7D6-DABF05F76CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAE4512-7A66-47AD-B9A9-AE45FF77F051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C92E99AE-170D-4566-9467-BE5E9489A7AF}"/>
   </bookViews>
@@ -563,7 +563,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -595,6 +595,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -914,7 +917,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -955,7 +958,7 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" t="b">
+      <c r="F2" s="11">
         <v>1</v>
       </c>
     </row>
@@ -972,7 +975,7 @@
       <c r="D3" s="2">
         <v>32</v>
       </c>
-      <c r="F3" t="b">
+      <c r="F3" s="11">
         <v>1</v>
       </c>
     </row>
@@ -989,7 +992,7 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" t="b">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1006,7 +1009,7 @@
       <c r="D5" s="2">
         <v>19</v>
       </c>
-      <c r="F5" t="b">
+      <c r="F5" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1023,7 +1026,7 @@
       <c r="D6" s="2">
         <v>11</v>
       </c>
-      <c r="F6" t="b">
+      <c r="F6" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1040,7 +1043,7 @@
       <c r="D7" s="2">
         <v>24</v>
       </c>
-      <c r="F7" t="b">
+      <c r="F7" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1057,7 +1060,7 @@
       <c r="D8" s="2">
         <v>11</v>
       </c>
-      <c r="F8" t="b">
+      <c r="F8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1074,7 +1077,7 @@
       <c r="D9" s="3">
         <v>84</v>
       </c>
-      <c r="F9" t="b">
+      <c r="F9" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1091,7 +1094,7 @@
       <c r="D10" s="2">
         <v>32</v>
       </c>
-      <c r="F10" t="b">
+      <c r="F10" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1108,7 +1111,7 @@
       <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" t="b">
+      <c r="F11" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1125,7 +1128,7 @@
       <c r="D12" s="2">
         <v>5</v>
       </c>
-      <c r="F12" t="b">
+      <c r="F12" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1142,7 +1145,7 @@
       <c r="D13" s="2">
         <v>11</v>
       </c>
-      <c r="F13" t="b">
+      <c r="F13" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1159,7 +1162,7 @@
       <c r="D14" s="2">
         <v>16</v>
       </c>
-      <c r="F14" t="b">
+      <c r="F14" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1176,7 +1179,7 @@
       <c r="D15" s="2">
         <v>5</v>
       </c>
-      <c r="F15" t="b">
+      <c r="F15" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1193,7 +1196,7 @@
       <c r="D16" s="2">
         <v>16</v>
       </c>
-      <c r="F16" t="b">
+      <c r="F16" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1210,7 +1213,7 @@
       <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="F17" t="b">
+      <c r="F17" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1227,7 +1230,7 @@
       <c r="D18" s="2">
         <v>11</v>
       </c>
-      <c r="F18" t="b">
+      <c r="F18" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1244,7 +1247,7 @@
       <c r="D19" s="2">
         <v>21</v>
       </c>
-      <c r="F19" t="b">
+      <c r="F19" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1261,7 +1264,7 @@
       <c r="D20" s="2">
         <v>19</v>
       </c>
-      <c r="F20" t="b">
+      <c r="F20" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1278,7 +1281,7 @@
       <c r="D21" s="2">
         <v>19</v>
       </c>
-      <c r="F21" t="b">
+      <c r="F21" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1295,7 +1298,7 @@
       <c r="D22" s="2">
         <v>77</v>
       </c>
-      <c r="F22" t="b">
+      <c r="F22" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1312,7 +1315,7 @@
       <c r="D23" s="2">
         <v>16</v>
       </c>
-      <c r="F23" t="b">
+      <c r="F23" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1329,7 +1332,7 @@
       <c r="D24" s="2">
         <v>11</v>
       </c>
-      <c r="F24" t="b">
+      <c r="F24" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1346,7 +1349,7 @@
       <c r="D25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F25" t="b">
+      <c r="F25" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1363,7 +1366,7 @@
       <c r="D26" s="2">
         <v>7</v>
       </c>
-      <c r="F26" t="b">
+      <c r="F26" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1380,7 +1383,7 @@
       <c r="D27" s="2">
         <v>16</v>
       </c>
-      <c r="F27" t="b">
+      <c r="F27" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1397,7 +1400,7 @@
       <c r="D28" s="2">
         <v>16</v>
       </c>
-      <c r="F28" t="b">
+      <c r="F28" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1414,7 +1417,7 @@
       <c r="D29" s="2">
         <v>0</v>
       </c>
-      <c r="F29" t="b">
+      <c r="F29" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1431,7 +1434,7 @@
       <c r="D30" s="2">
         <v>16</v>
       </c>
-      <c r="F30" t="b">
+      <c r="F30" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1448,7 +1451,7 @@
       <c r="D31" s="2">
         <v>11</v>
       </c>
-      <c r="F31" t="b">
+      <c r="F31" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1465,7 +1468,7 @@
       <c r="D32" s="2">
         <v>5</v>
       </c>
-      <c r="F32" t="b">
+      <c r="F32" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1482,7 +1485,7 @@
       <c r="D33" s="2">
         <v>32</v>
       </c>
-      <c r="F33" t="b">
+      <c r="F33" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1499,7 +1502,7 @@
       <c r="D34" s="2">
         <v>16</v>
       </c>
-      <c r="F34" t="b">
+      <c r="F34" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1516,7 +1519,7 @@
       <c r="D35" s="2">
         <v>0</v>
       </c>
-      <c r="F35" t="b">
+      <c r="F35" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1533,7 +1536,7 @@
       <c r="D36" s="2">
         <v>0</v>
       </c>
-      <c r="F36" t="b">
+      <c r="F36" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1550,7 +1553,7 @@
       <c r="D37" s="2">
         <v>11</v>
       </c>
-      <c r="F37" t="b">
+      <c r="F37" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1567,7 +1570,7 @@
       <c r="D38" s="2">
         <v>7</v>
       </c>
-      <c r="F38" t="b">
+      <c r="F38" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1584,7 +1587,7 @@
       <c r="D39" s="2">
         <v>0</v>
       </c>
-      <c r="F39" t="b">
+      <c r="F39" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1601,7 +1604,7 @@
       <c r="D40" s="2">
         <v>0</v>
       </c>
-      <c r="F40" t="b">
+      <c r="F40" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1618,7 +1621,7 @@
       <c r="D41" s="2">
         <v>0</v>
       </c>
-      <c r="F41" t="b">
+      <c r="F41" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1635,7 +1638,7 @@
       <c r="D42" s="2">
         <v>7</v>
       </c>
-      <c r="F42" t="b">
+      <c r="F42" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1652,7 +1655,7 @@
       <c r="D43" s="2">
         <v>16</v>
       </c>
-      <c r="F43" t="b">
+      <c r="F43" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1669,7 +1672,7 @@
       <c r="D44" s="2">
         <v>21</v>
       </c>
-      <c r="F44" t="b">
+      <c r="F44" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1686,7 +1689,7 @@
       <c r="D45" s="2">
         <v>26</v>
       </c>
-      <c r="F45" t="b">
+      <c r="F45" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1703,7 +1706,7 @@
       <c r="D46" s="2">
         <v>21</v>
       </c>
-      <c r="F46" t="b">
+      <c r="F46" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1720,7 +1723,7 @@
       <c r="D47" s="2">
         <v>0</v>
       </c>
-      <c r="F47" t="b">
+      <c r="F47" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1737,7 +1740,7 @@
       <c r="D48" s="2">
         <v>0</v>
       </c>
-      <c r="F48" t="b">
+      <c r="F48" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1754,7 +1757,7 @@
       <c r="D49" s="2">
         <v>0</v>
       </c>
-      <c r="F49" t="b">
+      <c r="F49" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1771,7 +1774,7 @@
       <c r="D50" s="2">
         <v>11</v>
       </c>
-      <c r="F50" t="b">
+      <c r="F50" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1788,7 +1791,7 @@
       <c r="D51" s="2">
         <v>16</v>
       </c>
-      <c r="F51" t="b">
+      <c r="F51" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1805,7 +1808,7 @@
       <c r="D52" s="2">
         <v>0</v>
       </c>
-      <c r="F52" t="b">
+      <c r="F52" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1822,7 +1825,7 @@
       <c r="D53" s="5">
         <v>42</v>
       </c>
-      <c r="F53" t="b">
+      <c r="F53" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1836,7 +1839,7 @@
       <c r="E54" t="s">
         <v>67</v>
       </c>
-      <c r="F54" t="b">
+      <c r="F54">
         <v>0</v>
       </c>
     </row>
@@ -1850,7 +1853,7 @@
       <c r="E55" t="s">
         <v>67</v>
       </c>
-      <c r="F55" t="b">
+      <c r="F55">
         <v>0</v>
       </c>
     </row>
@@ -1864,7 +1867,7 @@
       <c r="E56" t="s">
         <v>67</v>
       </c>
-      <c r="F56" t="b">
+      <c r="F56">
         <v>0</v>
       </c>
     </row>
@@ -1878,7 +1881,7 @@
       <c r="E57" t="s">
         <v>67</v>
       </c>
-      <c r="F57" t="b">
+      <c r="F57">
         <v>0</v>
       </c>
     </row>
@@ -1892,7 +1895,7 @@
       <c r="E58" t="s">
         <v>67</v>
       </c>
-      <c r="F58" t="b">
+      <c r="F58">
         <v>0</v>
       </c>
     </row>
@@ -1906,7 +1909,7 @@
       <c r="E59" t="s">
         <v>67</v>
       </c>
-      <c r="F59" t="b">
+      <c r="F59">
         <v>0</v>
       </c>
     </row>
@@ -1920,7 +1923,7 @@
       <c r="E60" t="s">
         <v>67</v>
       </c>
-      <c r="F60" t="b">
+      <c r="F60">
         <v>0</v>
       </c>
     </row>
@@ -1934,7 +1937,7 @@
       <c r="E61" t="s">
         <v>67</v>
       </c>
-      <c r="F61" t="b">
+      <c r="F61">
         <v>0</v>
       </c>
     </row>
@@ -1948,7 +1951,7 @@
       <c r="E62" t="s">
         <v>67</v>
       </c>
-      <c r="F62" t="b">
+      <c r="F62">
         <v>0</v>
       </c>
     </row>
@@ -1962,7 +1965,7 @@
       <c r="E63" t="s">
         <v>67</v>
       </c>
-      <c r="F63" t="b">
+      <c r="F63">
         <v>0</v>
       </c>
     </row>
@@ -1976,7 +1979,7 @@
       <c r="E64" t="s">
         <v>67</v>
       </c>
-      <c r="F64" t="b">
+      <c r="F64">
         <v>0</v>
       </c>
     </row>
@@ -1990,7 +1993,7 @@
       <c r="E65" t="s">
         <v>67</v>
       </c>
-      <c r="F65" t="b">
+      <c r="F65">
         <v>0</v>
       </c>
     </row>
@@ -2004,7 +2007,7 @@
       <c r="E66" t="s">
         <v>67</v>
       </c>
-      <c r="F66" t="b">
+      <c r="F66">
         <v>0</v>
       </c>
     </row>
@@ -2018,7 +2021,7 @@
       <c r="E67" t="s">
         <v>66</v>
       </c>
-      <c r="F67" t="b">
+      <c r="F67">
         <v>0</v>
       </c>
     </row>
@@ -2032,7 +2035,7 @@
       <c r="E68" t="s">
         <v>66</v>
       </c>
-      <c r="F68" t="b">
+      <c r="F68">
         <v>0</v>
       </c>
     </row>
@@ -2046,7 +2049,7 @@
       <c r="E69" t="s">
         <v>66</v>
       </c>
-      <c r="F69" t="b">
+      <c r="F69">
         <v>0</v>
       </c>
     </row>
@@ -2060,7 +2063,7 @@
       <c r="E70" t="s">
         <v>66</v>
       </c>
-      <c r="F70" t="b">
+      <c r="F70">
         <v>0</v>
       </c>
     </row>
@@ -2074,7 +2077,7 @@
       <c r="E71" t="s">
         <v>73</v>
       </c>
-      <c r="F71" t="b">
+      <c r="F71">
         <v>0</v>
       </c>
     </row>
@@ -2088,7 +2091,7 @@
       <c r="E72" t="s">
         <v>73</v>
       </c>
-      <c r="F72" t="b">
+      <c r="F72">
         <v>0</v>
       </c>
     </row>
@@ -2102,7 +2105,7 @@
       <c r="E73" t="s">
         <v>73</v>
       </c>
-      <c r="F73" t="b">
+      <c r="F73">
         <v>0</v>
       </c>
     </row>
@@ -2116,7 +2119,7 @@
       <c r="E74" t="s">
         <v>73</v>
       </c>
-      <c r="F74" t="b">
+      <c r="F74">
         <v>0</v>
       </c>
     </row>
@@ -2130,7 +2133,7 @@
       <c r="E75" t="s">
         <v>73</v>
       </c>
-      <c r="F75" t="b">
+      <c r="F75">
         <v>0</v>
       </c>
     </row>
@@ -2144,7 +2147,7 @@
       <c r="E76" t="s">
         <v>73</v>
       </c>
-      <c r="F76" t="b">
+      <c r="F76">
         <v>0</v>
       </c>
     </row>
@@ -2158,7 +2161,7 @@
       <c r="E77" t="s">
         <v>73</v>
       </c>
-      <c r="F77" t="b">
+      <c r="F77">
         <v>0</v>
       </c>
     </row>
@@ -2172,7 +2175,7 @@
       <c r="E78" t="s">
         <v>73</v>
       </c>
-      <c r="F78" t="b">
+      <c r="F78">
         <v>0</v>
       </c>
     </row>
@@ -2186,7 +2189,7 @@
       <c r="E79" t="s">
         <v>73</v>
       </c>
-      <c r="F79" t="b">
+      <c r="F79">
         <v>0</v>
       </c>
     </row>
@@ -2200,7 +2203,7 @@
       <c r="E80" t="s">
         <v>73</v>
       </c>
-      <c r="F80" t="b">
+      <c r="F80">
         <v>0</v>
       </c>
     </row>
@@ -2214,7 +2217,7 @@
       <c r="E81" t="s">
         <v>73</v>
       </c>
-      <c r="F81" t="b">
+      <c r="F81">
         <v>0</v>
       </c>
     </row>
@@ -2228,7 +2231,7 @@
       <c r="E82" t="s">
         <v>73</v>
       </c>
-      <c r="F82" t="b">
+      <c r="F82">
         <v>0</v>
       </c>
     </row>
@@ -2242,7 +2245,7 @@
       <c r="E83" t="s">
         <v>73</v>
       </c>
-      <c r="F83" t="b">
+      <c r="F83">
         <v>0</v>
       </c>
     </row>
@@ -2256,7 +2259,7 @@
       <c r="E84" t="s">
         <v>73</v>
       </c>
-      <c r="F84" t="b">
+      <c r="F84">
         <v>0</v>
       </c>
     </row>
@@ -2270,7 +2273,7 @@
       <c r="E85" t="s">
         <v>73</v>
       </c>
-      <c r="F85" t="b">
+      <c r="F85">
         <v>0</v>
       </c>
     </row>
@@ -2284,7 +2287,7 @@
       <c r="E86" t="s">
         <v>73</v>
       </c>
-      <c r="F86" t="b">
+      <c r="F86">
         <v>0</v>
       </c>
     </row>
@@ -2298,7 +2301,7 @@
       <c r="E87" t="s">
         <v>73</v>
       </c>
-      <c r="F87" t="b">
+      <c r="F87">
         <v>0</v>
       </c>
     </row>
@@ -2312,7 +2315,7 @@
       <c r="E88" t="s">
         <v>73</v>
       </c>
-      <c r="F88" t="b">
+      <c r="F88">
         <v>0</v>
       </c>
     </row>
@@ -2326,7 +2329,7 @@
       <c r="E89" t="s">
         <v>73</v>
       </c>
-      <c r="F89" t="b">
+      <c r="F89">
         <v>0</v>
       </c>
     </row>

</xml_diff>